<commit_message>
WIP: Implementing control/cell value sync feature
</commit_message>
<xml_diff>
--- a/testcases/test-data/spreadsheet/WithControl.xlsx
+++ b/testcases/test-data/spreadsheet/WithControl.xlsx
@@ -126,15 +126,27 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" firstButton="1" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" firstButton="1" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$C$14" fmlaRange="$I$6:$K$8" noThreeD="1" sel="3" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="GBox" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" firstButton="1" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -354,6 +366,186 @@
               <a:avLst/>
             </a:prstGeom>
           </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>666750</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="Group Box 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="none" lIns="27432" tIns="18288" rIns="0" bIns="0" anchor="t" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="ja-JP" altLang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="MS UI Gothic"/>
+                  <a:ea typeface="MS UI Gothic"/>
+                </a:rPr>
+                <a:t>グループ 5</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>600075</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1030" name="Option Button 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1030"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="ja-JP" altLang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="MS UI Gothic"/>
+                  <a:ea typeface="MS UI Gothic"/>
+                </a:rPr>
+                <a:t>オプション 6</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>133350</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>304800</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1031" name="Option Button 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1031"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="ja-JP" altLang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="MS UI Gothic"/>
+                  <a:ea typeface="MS UI Gothic"/>
+                </a:rPr>
+                <a:t>オプション 7</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
       </xdr:twoCellAnchor>
@@ -653,7 +845,7 @@
   <dimension ref="C4:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -693,7 +885,7 @@
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1">
         <v>1</v>
@@ -807,6 +999,72 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1029" r:id="rId8" name="Group Box 5">
+              <controlPr defaultSize="0" autoFill="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>666750</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>8</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1030" r:id="rId9" name="Option Button 6">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>24</xdr:row>
+                    <xdr:rowOff>76200</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>600075</xdr:colOff>
+                    <xdr:row>26</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1031" r:id="rId10" name="Option Button 7">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>133350</xdr:colOff>
+                    <xdr:row>24</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>304800</xdr:colOff>
+                    <xdr:row>26</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>

</xml_diff>